<commit_message>
updated bibtex data and pdf
</commit_message>
<xml_diff>
--- a/stats/data/data_dv.xlsx
+++ b/stats/data/data_dv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janetbang/Dropbox/Other_Research/2019_socpop/SocPop/stats/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3AB33A-744F-1A49-BF14-B936CE5399B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D7D304-31FD-614C-A56E-29845659A00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="780" windowWidth="30460" windowHeight="19180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_children_n43" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="26">
   <si>
     <t>id</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>L1PRE_PS_AWChr</t>
-  </si>
-  <si>
-    <t>L1POST_hi</t>
   </si>
   <si>
     <t>L1POST_cdi_version</t>
@@ -944,24 +941,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S43"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="8" max="8" width="10.83203125" customWidth="1"/>
-    <col min="10" max="12" width="10.83203125" customWidth="1"/>
-    <col min="14" max="14" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.5" customWidth="1"/>
-    <col min="16" max="17" width="14.83203125" customWidth="1"/>
-    <col min="18" max="18" width="16.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="9" max="11" width="10.83203125" customWidth="1"/>
+    <col min="13" max="13" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.5" customWidth="1"/>
+    <col min="15" max="16" width="14.83203125" customWidth="1"/>
+    <col min="17" max="17" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -978,22 +975,22 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
         <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
       </c>
       <c r="L1" t="s">
         <v>12</v>
@@ -1005,24 +1002,21 @@
         <v>14</v>
       </c>
       <c r="O1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="P1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R1" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R1" t="s">
-        <v>10</v>
-      </c>
-      <c r="S1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>18.600000000000001</v>
@@ -1037,49 +1031,46 @@
         <v>24</v>
       </c>
       <c r="F2">
-        <v>24</v>
-      </c>
-      <c r="G2">
         <v>0</v>
       </c>
-      <c r="H2" t="s">
-        <v>16</v>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <v>33</v>
       </c>
       <c r="I2">
-        <v>33</v>
+        <v>0.67876115400000003</v>
       </c>
       <c r="J2">
-        <v>0.67876115400000003</v>
-      </c>
-      <c r="K2">
         <v>1258.5</v>
       </c>
-      <c r="L2" t="s">
-        <v>17</v>
+      <c r="K2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2">
+        <v>292</v>
       </c>
       <c r="M2">
-        <v>292</v>
+        <v>0.50486514800000004</v>
       </c>
       <c r="N2">
-        <v>0.50486514800000004</v>
+        <v>889.45454549999999</v>
       </c>
       <c r="O2">
-        <v>889.45454549999999</v>
+        <v>11</v>
       </c>
       <c r="P2">
-        <v>11</v>
+        <v>326.90804930000002</v>
       </c>
       <c r="Q2">
-        <v>326.90804930000002</v>
-      </c>
-      <c r="R2">
         <v>4020.5391530000002</v>
       </c>
-      <c r="S2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>105</v>
       </c>
@@ -1096,49 +1087,46 @@
         <v>37.5</v>
       </c>
       <c r="F3">
-        <v>25</v>
-      </c>
-      <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3" t="s">
-        <v>16</v>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3">
+        <v>43</v>
       </c>
       <c r="I3">
-        <v>43</v>
+        <v>0.49232948100000001</v>
       </c>
       <c r="J3">
-        <v>0.49232948100000001</v>
-      </c>
-      <c r="K3">
         <v>1138.8888890000001</v>
       </c>
-      <c r="L3" t="s">
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3">
+        <v>124</v>
+      </c>
+      <c r="M3">
+        <v>0.60283268999999995</v>
+      </c>
+      <c r="N3">
+        <v>1010.823529</v>
+      </c>
+      <c r="O3">
         <v>17</v>
       </c>
-      <c r="M3">
-        <v>124</v>
-      </c>
-      <c r="N3">
-        <v>0.60283268999999995</v>
-      </c>
-      <c r="O3">
-        <v>1010.823529</v>
-      </c>
       <c r="P3">
-        <v>17</v>
+        <v>401.80829310000001</v>
       </c>
       <c r="Q3">
-        <v>401.80829310000001</v>
-      </c>
-      <c r="R3">
         <v>5471.3826369999997</v>
       </c>
-      <c r="S3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>109</v>
       </c>
@@ -1155,49 +1143,46 @@
         <v>19.5</v>
       </c>
       <c r="F4">
-        <v>19.5</v>
-      </c>
-      <c r="G4">
         <v>0</v>
       </c>
-      <c r="H4" t="s">
-        <v>16</v>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4">
+        <v>140</v>
       </c>
       <c r="I4">
-        <v>140</v>
+        <v>0.42237707499999999</v>
       </c>
       <c r="J4">
-        <v>0.42237707499999999</v>
-      </c>
-      <c r="K4">
         <v>961.85714289999999</v>
       </c>
-      <c r="L4" t="s">
-        <v>17</v>
+      <c r="K4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4">
+        <v>355</v>
       </c>
       <c r="M4">
-        <v>355</v>
+        <v>0.71522216199999999</v>
       </c>
       <c r="N4">
-        <v>0.71522216199999999</v>
+        <v>664.2142857</v>
       </c>
       <c r="O4">
-        <v>664.2142857</v>
+        <v>14</v>
       </c>
       <c r="P4">
-        <v>14</v>
+        <v>205.70598079999999</v>
       </c>
       <c r="Q4">
-        <v>205.70598079999999</v>
-      </c>
-      <c r="R4">
         <v>5550.7614210000002</v>
       </c>
-      <c r="S4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>114</v>
       </c>
@@ -1214,49 +1199,46 @@
         <v>22.5</v>
       </c>
       <c r="F5">
-        <v>21</v>
-      </c>
-      <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5" t="s">
-        <v>16</v>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <v>9</v>
       </c>
       <c r="I5">
-        <v>9</v>
+        <v>0.59977146400000003</v>
       </c>
       <c r="J5">
-        <v>0.59977146400000003</v>
-      </c>
-      <c r="K5">
         <v>884.72727269999996</v>
       </c>
-      <c r="L5" t="s">
-        <v>17</v>
+      <c r="K5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5">
+        <v>139</v>
       </c>
       <c r="M5">
-        <v>139</v>
+        <v>0.65706330599999996</v>
       </c>
       <c r="N5">
-        <v>0.65706330599999996</v>
+        <v>889.5625</v>
       </c>
       <c r="O5">
-        <v>889.5625</v>
+        <v>16</v>
       </c>
       <c r="P5">
-        <v>16</v>
+        <v>287.37408110000001</v>
       </c>
       <c r="Q5">
-        <v>287.37408110000001</v>
-      </c>
-      <c r="R5">
         <v>2953.6159600000001</v>
       </c>
-      <c r="S5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>121</v>
       </c>
@@ -1273,49 +1255,46 @@
         <v>22</v>
       </c>
       <c r="F6">
-        <v>27</v>
-      </c>
-      <c r="G6">
         <v>1</v>
       </c>
-      <c r="H6" t="s">
-        <v>16</v>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>0.62476485500000001</v>
       </c>
       <c r="J6">
-        <v>0.62476485500000001</v>
-      </c>
-      <c r="K6">
         <v>647.33333330000005</v>
       </c>
-      <c r="L6" t="s">
-        <v>17</v>
+      <c r="K6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6">
+        <v>347</v>
       </c>
       <c r="M6">
-        <v>347</v>
+        <v>0.67391723400000003</v>
       </c>
       <c r="N6">
-        <v>0.67391723400000003</v>
+        <v>863.3</v>
       </c>
       <c r="O6">
-        <v>863.3</v>
+        <v>10</v>
       </c>
       <c r="P6">
-        <v>10</v>
+        <v>264.31338720000002</v>
       </c>
       <c r="Q6">
-        <v>264.31338720000002</v>
-      </c>
-      <c r="R6">
         <v>2554.83871</v>
       </c>
-      <c r="S6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>132</v>
       </c>
@@ -1332,49 +1311,46 @@
         <v>40</v>
       </c>
       <c r="F7">
-        <v>40</v>
-      </c>
-      <c r="G7">
         <v>0</v>
       </c>
-      <c r="H7" t="s">
-        <v>16</v>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7">
+        <v>67</v>
       </c>
       <c r="I7">
-        <v>67</v>
+        <v>0.722596444</v>
       </c>
       <c r="J7">
-        <v>0.722596444</v>
-      </c>
-      <c r="K7">
         <v>916.6</v>
       </c>
-      <c r="L7" t="s">
-        <v>17</v>
+      <c r="K7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7">
+        <v>446</v>
       </c>
       <c r="M7">
-        <v>446</v>
+        <v>0.513843622</v>
       </c>
       <c r="N7">
-        <v>0.513843622</v>
+        <v>726.11111110000002</v>
       </c>
       <c r="O7">
-        <v>726.11111110000002</v>
+        <v>9</v>
       </c>
       <c r="P7">
-        <v>9</v>
+        <v>160.0729868</v>
       </c>
       <c r="Q7">
-        <v>160.0729868</v>
-      </c>
-      <c r="R7">
         <v>4118.2165610000002</v>
       </c>
-      <c r="S7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>133</v>
       </c>
@@ -1391,49 +1367,46 @@
         <v>27</v>
       </c>
       <c r="F8">
-        <v>24.5</v>
-      </c>
-      <c r="G8">
         <v>0</v>
       </c>
-      <c r="H8" t="s">
-        <v>16</v>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
       </c>
       <c r="I8">
-        <v>2</v>
+        <v>0.55322591899999995</v>
       </c>
       <c r="J8">
-        <v>0.55322591899999995</v>
-      </c>
-      <c r="K8">
         <v>691.75</v>
       </c>
-      <c r="L8" t="s">
-        <v>17</v>
+      <c r="K8" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8">
+        <v>252</v>
       </c>
       <c r="M8">
-        <v>252</v>
+        <v>0.458336731</v>
       </c>
       <c r="N8">
-        <v>0.458336731</v>
+        <v>1083.25</v>
       </c>
       <c r="O8">
-        <v>1083.25</v>
+        <v>4</v>
       </c>
       <c r="P8">
-        <v>4</v>
+        <v>513.72649990000002</v>
       </c>
       <c r="Q8">
-        <v>513.72649990000002</v>
-      </c>
-      <c r="R8">
         <v>3428.1290319999998</v>
       </c>
-      <c r="S8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>140</v>
       </c>
@@ -1450,49 +1423,46 @@
         <v>17.5</v>
       </c>
       <c r="F9">
-        <v>17.5</v>
-      </c>
-      <c r="G9">
         <v>1</v>
       </c>
-      <c r="H9" t="s">
-        <v>16</v>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <v>166</v>
       </c>
       <c r="I9">
-        <v>166</v>
+        <v>0.548811049</v>
       </c>
       <c r="J9">
-        <v>0.548811049</v>
-      </c>
-      <c r="K9">
         <v>1115.25</v>
       </c>
-      <c r="L9" t="s">
-        <v>17</v>
+      <c r="K9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9">
+        <v>280</v>
       </c>
       <c r="M9">
-        <v>280</v>
+        <v>0.67913470099999995</v>
       </c>
       <c r="N9">
-        <v>0.67913470099999995</v>
+        <v>743.53846150000004</v>
       </c>
       <c r="O9">
-        <v>743.53846150000004</v>
+        <v>13</v>
       </c>
       <c r="P9">
-        <v>13</v>
+        <v>228.18582169999999</v>
       </c>
       <c r="Q9">
-        <v>228.18582169999999</v>
-      </c>
-      <c r="R9">
         <v>3377.419355</v>
       </c>
-      <c r="S9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>141</v>
       </c>
@@ -1509,49 +1479,46 @@
         <v>20</v>
       </c>
       <c r="F10">
-        <v>24</v>
-      </c>
-      <c r="G10">
         <v>1</v>
       </c>
-      <c r="H10" t="s">
-        <v>16</v>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10">
+        <v>6</v>
       </c>
       <c r="I10">
-        <v>6</v>
+        <v>0.60060562299999998</v>
       </c>
       <c r="J10">
-        <v>0.60060562299999998</v>
-      </c>
-      <c r="K10">
         <v>916.5</v>
       </c>
-      <c r="L10" t="s">
-        <v>17</v>
+      <c r="K10" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10">
+        <v>525</v>
       </c>
       <c r="M10">
-        <v>525</v>
+        <v>0.72870429000000003</v>
       </c>
       <c r="N10">
-        <v>0.72870429000000003</v>
+        <v>841.75</v>
       </c>
       <c r="O10">
-        <v>841.75</v>
+        <v>4</v>
       </c>
       <c r="P10">
-        <v>4</v>
+        <v>317.95951000000002</v>
       </c>
       <c r="Q10">
-        <v>317.95951000000002</v>
-      </c>
-      <c r="R10">
         <v>5738.9473680000001</v>
       </c>
-      <c r="S10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>145</v>
       </c>
@@ -1568,49 +1535,46 @@
         <v>28</v>
       </c>
       <c r="F11">
-        <v>25.5</v>
-      </c>
-      <c r="G11">
         <v>1</v>
       </c>
-      <c r="H11" t="s">
-        <v>16</v>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11">
+        <v>163</v>
       </c>
       <c r="I11">
-        <v>163</v>
+        <v>0.71023524400000004</v>
       </c>
       <c r="J11">
-        <v>0.71023524400000004</v>
-      </c>
-      <c r="K11">
         <v>605.5</v>
       </c>
-      <c r="L11" t="s">
-        <v>17</v>
+      <c r="K11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L11">
+        <v>410</v>
       </c>
       <c r="M11">
-        <v>410</v>
+        <v>0.77338536499999999</v>
       </c>
       <c r="N11">
-        <v>0.77338536499999999</v>
+        <v>547</v>
       </c>
       <c r="O11">
-        <v>547</v>
+        <v>16</v>
       </c>
       <c r="P11">
-        <v>16</v>
+        <v>139.98190360000001</v>
       </c>
       <c r="Q11">
-        <v>139.98190360000001</v>
-      </c>
-      <c r="R11">
         <v>3713.8686130000001</v>
       </c>
-      <c r="S11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>146</v>
       </c>
@@ -1627,49 +1591,46 @@
         <v>29.5</v>
       </c>
       <c r="F12">
-        <v>27</v>
-      </c>
-      <c r="G12">
         <v>0</v>
       </c>
-      <c r="H12" t="s">
-        <v>16</v>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>0.49611754499999999</v>
       </c>
       <c r="J12">
-        <v>0.49611754499999999</v>
-      </c>
-      <c r="K12">
         <v>855.5</v>
       </c>
-      <c r="L12" t="s">
-        <v>17</v>
+      <c r="K12" t="s">
+        <v>16</v>
+      </c>
+      <c r="L12">
+        <v>24</v>
       </c>
       <c r="M12">
-        <v>24</v>
+        <v>0.71262498200000002</v>
       </c>
       <c r="N12">
-        <v>0.71262498200000002</v>
+        <v>629.38095239999996</v>
       </c>
       <c r="O12">
-        <v>629.38095239999996</v>
+        <v>21</v>
       </c>
       <c r="P12">
-        <v>21</v>
+        <v>201.1972853</v>
       </c>
       <c r="Q12">
-        <v>201.1972853</v>
-      </c>
-      <c r="R12">
         <v>2688.2778579999999</v>
       </c>
-      <c r="S12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>150</v>
       </c>
@@ -1686,49 +1647,46 @@
         <v>13</v>
       </c>
       <c r="F13">
-        <v>13</v>
-      </c>
-      <c r="G13">
         <v>1</v>
       </c>
-      <c r="H13" t="s">
-        <v>16</v>
+      <c r="G13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>0.60801108100000001</v>
       </c>
       <c r="J13">
-        <v>0.60801108100000001</v>
-      </c>
-      <c r="K13">
         <v>1025</v>
       </c>
-      <c r="L13" t="s">
-        <v>17</v>
+      <c r="K13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L13">
+        <v>567</v>
       </c>
       <c r="M13">
-        <v>567</v>
+        <v>0.57697115600000004</v>
       </c>
       <c r="N13">
-        <v>0.57697115600000004</v>
+        <v>937</v>
       </c>
       <c r="O13">
-        <v>937</v>
+        <v>9</v>
       </c>
       <c r="P13">
-        <v>9</v>
+        <v>256.03320100000002</v>
       </c>
       <c r="Q13">
-        <v>256.03320100000002</v>
-      </c>
-      <c r="R13">
         <v>4842.0233459999999</v>
       </c>
-      <c r="S13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>157</v>
       </c>
@@ -1745,49 +1703,46 @@
         <v>24</v>
       </c>
       <c r="F14">
-        <v>18.5</v>
-      </c>
-      <c r="G14">
         <v>1</v>
       </c>
-      <c r="H14" t="s">
-        <v>16</v>
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14">
+        <v>246</v>
       </c>
       <c r="I14">
-        <v>246</v>
+        <v>0.54607054200000005</v>
       </c>
       <c r="J14">
-        <v>0.54607054200000005</v>
-      </c>
-      <c r="K14">
         <v>975</v>
       </c>
-      <c r="L14" t="s">
-        <v>17</v>
+      <c r="K14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14">
+        <v>588</v>
       </c>
       <c r="M14">
-        <v>588</v>
+        <v>0.58774779200000005</v>
       </c>
       <c r="N14">
-        <v>0.58774779200000005</v>
+        <v>781.44444439999995</v>
       </c>
       <c r="O14">
-        <v>781.44444439999995</v>
+        <v>9</v>
       </c>
       <c r="P14">
-        <v>9</v>
+        <v>299.19605239999999</v>
       </c>
       <c r="Q14">
-        <v>299.19605239999999</v>
-      </c>
-      <c r="R14">
         <v>4998.7819730000001</v>
       </c>
-      <c r="S14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>168</v>
       </c>
@@ -1804,49 +1759,46 @@
         <v>13</v>
       </c>
       <c r="F15">
-        <v>23.5</v>
-      </c>
-      <c r="G15">
         <v>1</v>
       </c>
-      <c r="H15" t="s">
-        <v>16</v>
+      <c r="G15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15">
+        <v>8</v>
       </c>
       <c r="I15">
-        <v>8</v>
+        <v>0.68801091700000006</v>
       </c>
       <c r="J15">
-        <v>0.68801091700000006</v>
-      </c>
-      <c r="K15">
         <v>767</v>
       </c>
-      <c r="L15" t="s">
+      <c r="K15" t="s">
+        <v>16</v>
+      </c>
+      <c r="L15">
+        <v>474</v>
+      </c>
+      <c r="M15">
+        <v>0.63041758800000003</v>
+      </c>
+      <c r="N15">
+        <v>921.58823529999995</v>
+      </c>
+      <c r="O15">
         <v>17</v>
       </c>
-      <c r="M15">
-        <v>474</v>
-      </c>
-      <c r="N15">
-        <v>0.63041758800000003</v>
-      </c>
-      <c r="O15">
-        <v>921.58823529999995</v>
-      </c>
       <c r="P15">
-        <v>17</v>
+        <v>388.51304010000001</v>
       </c>
       <c r="Q15">
-        <v>388.51304010000001</v>
-      </c>
-      <c r="R15">
         <v>4501.1920529999998</v>
       </c>
-      <c r="S15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>182</v>
       </c>
@@ -1863,49 +1815,46 @@
         <v>27</v>
       </c>
       <c r="F16">
-        <v>19</v>
-      </c>
-      <c r="G16">
         <v>1</v>
       </c>
-      <c r="H16" t="s">
-        <v>16</v>
+      <c r="G16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16">
+        <v>7</v>
       </c>
       <c r="I16">
-        <v>7</v>
+        <v>0.70463935099999997</v>
       </c>
       <c r="J16">
-        <v>0.70463935099999997</v>
-      </c>
-      <c r="K16">
         <v>616.79999999999995</v>
       </c>
-      <c r="L16" t="s">
-        <v>17</v>
+      <c r="K16" t="s">
+        <v>16</v>
+      </c>
+      <c r="L16">
+        <v>41</v>
       </c>
       <c r="M16">
-        <v>41</v>
+        <v>0.66031555399999997</v>
       </c>
       <c r="N16">
-        <v>0.66031555399999997</v>
+        <v>866.66666669999995</v>
       </c>
       <c r="O16">
-        <v>866.66666669999995</v>
+        <v>12</v>
       </c>
       <c r="P16">
-        <v>12</v>
+        <v>300.2996483</v>
       </c>
       <c r="Q16">
-        <v>300.2996483</v>
-      </c>
-      <c r="R16">
         <v>5384.2302879999997</v>
       </c>
-      <c r="S16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>190</v>
       </c>
@@ -1922,47 +1871,44 @@
         <v>29</v>
       </c>
       <c r="F17">
-        <v>29</v>
-      </c>
-      <c r="G17">
         <v>0</v>
       </c>
-      <c r="H17" t="s">
-        <v>16</v>
+      <c r="G17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17">
+        <v>4</v>
       </c>
       <c r="I17">
-        <v>4</v>
+        <v>0.618792538</v>
       </c>
       <c r="J17">
-        <v>0.618792538</v>
-      </c>
-      <c r="K17">
         <v>795.2857143</v>
       </c>
-      <c r="L17" t="s">
-        <v>17</v>
-      </c>
-      <c r="M17" s="3"/>
+      <c r="K17" t="s">
+        <v>16</v>
+      </c>
+      <c r="L17" s="3"/>
+      <c r="M17">
+        <v>0.63768814200000001</v>
+      </c>
       <c r="N17">
-        <v>0.63768814200000001</v>
+        <v>938.77777779999997</v>
       </c>
       <c r="O17">
-        <v>938.77777779999997</v>
+        <v>9</v>
       </c>
       <c r="P17">
-        <v>9</v>
+        <v>323.79267199999998</v>
       </c>
       <c r="Q17">
-        <v>323.79267199999998</v>
-      </c>
-      <c r="R17">
         <v>3975.8490569999999</v>
       </c>
-      <c r="S17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>192</v>
       </c>
@@ -1979,49 +1925,46 @@
         <v>45</v>
       </c>
       <c r="F18">
-        <v>44</v>
-      </c>
-      <c r="G18">
         <v>1</v>
       </c>
-      <c r="H18" t="s">
-        <v>16</v>
+      <c r="G18" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18">
+        <v>132</v>
       </c>
       <c r="I18">
-        <v>132</v>
+        <v>0.54028765300000003</v>
       </c>
       <c r="J18">
-        <v>0.54028765300000003</v>
-      </c>
-      <c r="K18">
         <v>1032</v>
       </c>
-      <c r="L18" t="s">
-        <v>17</v>
-      </c>
-      <c r="M18" s="3">
+      <c r="K18" t="s">
+        <v>16</v>
+      </c>
+      <c r="L18" s="3">
         <v>467</v>
       </c>
+      <c r="M18">
+        <v>0.665611693</v>
+      </c>
       <c r="N18">
-        <v>0.665611693</v>
+        <v>627</v>
       </c>
       <c r="O18">
-        <v>627</v>
+        <v>13</v>
       </c>
       <c r="P18">
-        <v>13</v>
+        <v>177.3339599</v>
       </c>
       <c r="Q18">
-        <v>177.3339599</v>
-      </c>
-      <c r="R18">
         <v>4746.3976949999997</v>
       </c>
-      <c r="S18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>193</v>
       </c>
@@ -2038,47 +1981,44 @@
         <v>15.5</v>
       </c>
       <c r="F19">
-        <v>12.5</v>
-      </c>
-      <c r="G19">
         <v>1</v>
       </c>
-      <c r="H19" t="s">
-        <v>16</v>
+      <c r="G19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
       </c>
       <c r="I19">
-        <v>4</v>
+        <v>0.60688467599999996</v>
       </c>
       <c r="J19">
-        <v>0.60688467599999996</v>
-      </c>
-      <c r="K19">
         <v>1037.1111109999999</v>
       </c>
-      <c r="L19" t="s">
-        <v>17</v>
-      </c>
-      <c r="M19" s="3"/>
+      <c r="K19" t="s">
+        <v>16</v>
+      </c>
+      <c r="L19" s="3"/>
+      <c r="M19">
+        <v>0.66929529600000004</v>
+      </c>
       <c r="N19">
-        <v>0.66929529600000004</v>
+        <v>844.8125</v>
       </c>
       <c r="O19">
-        <v>844.8125</v>
+        <v>16</v>
       </c>
       <c r="P19">
-        <v>16</v>
+        <v>311.07024259999997</v>
       </c>
       <c r="Q19">
-        <v>311.07024259999997</v>
-      </c>
-      <c r="R19">
         <v>1173.81258</v>
       </c>
-      <c r="S19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>196</v>
       </c>
@@ -2095,49 +2035,46 @@
         <v>43</v>
       </c>
       <c r="F20">
-        <v>43</v>
-      </c>
-      <c r="G20">
         <v>1</v>
       </c>
-      <c r="H20" t="s">
-        <v>16</v>
+      <c r="G20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20">
+        <v>41</v>
       </c>
       <c r="I20">
-        <v>41</v>
+        <v>0.68635321100000002</v>
       </c>
       <c r="J20">
-        <v>0.68635321100000002</v>
-      </c>
-      <c r="K20">
         <v>888.66666669999995</v>
       </c>
-      <c r="L20" t="s">
-        <v>17</v>
-      </c>
-      <c r="M20" s="3">
+      <c r="K20" t="s">
+        <v>16</v>
+      </c>
+      <c r="L20" s="3">
         <v>153</v>
       </c>
+      <c r="M20">
+        <v>0.71919685300000002</v>
+      </c>
       <c r="N20">
-        <v>0.71919685300000002</v>
+        <v>656.46153849999996</v>
       </c>
       <c r="O20">
-        <v>656.46153849999996</v>
+        <v>13</v>
       </c>
       <c r="P20">
-        <v>13</v>
+        <v>289.80873450000001</v>
       </c>
       <c r="Q20">
-        <v>289.80873450000001</v>
-      </c>
-      <c r="R20">
         <v>3028.0373829999999</v>
       </c>
-      <c r="S20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>197</v>
       </c>
@@ -2154,49 +2091,46 @@
         <v>20</v>
       </c>
       <c r="F21">
-        <v>18.5</v>
-      </c>
-      <c r="G21">
         <v>0</v>
       </c>
-      <c r="H21" t="s">
+      <c r="G21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21">
         <v>16</v>
       </c>
       <c r="I21">
-        <v>16</v>
+        <v>0.51167870999999998</v>
       </c>
       <c r="J21">
-        <v>0.51167870999999998</v>
-      </c>
-      <c r="K21">
         <v>1065</v>
       </c>
-      <c r="L21" t="s">
-        <v>17</v>
-      </c>
-      <c r="M21" s="3">
+      <c r="K21" t="s">
+        <v>16</v>
+      </c>
+      <c r="L21" s="3">
         <v>22</v>
       </c>
+      <c r="M21">
+        <v>0.62887712399999995</v>
+      </c>
       <c r="N21">
-        <v>0.62887712399999995</v>
+        <v>1046.8</v>
       </c>
       <c r="O21">
-        <v>1046.8</v>
+        <v>5</v>
       </c>
       <c r="P21">
-        <v>5</v>
+        <v>402.90408289999999</v>
       </c>
       <c r="Q21">
-        <v>402.90408289999999</v>
-      </c>
-      <c r="R21">
         <v>712.95843520000005</v>
       </c>
-      <c r="S21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>232</v>
       </c>
@@ -2213,49 +2147,46 @@
         <v>24</v>
       </c>
       <c r="F22">
-        <v>21.5</v>
-      </c>
-      <c r="G22">
         <v>0</v>
       </c>
-      <c r="H22" t="s">
-        <v>17</v>
+      <c r="G22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22">
+        <v>31</v>
       </c>
       <c r="I22">
-        <v>31</v>
+        <v>0.53801933999999996</v>
       </c>
       <c r="J22">
-        <v>0.53801933999999996</v>
-      </c>
-      <c r="K22">
         <v>997.53846150000004</v>
       </c>
-      <c r="L22" t="s">
-        <v>17</v>
-      </c>
-      <c r="M22" s="3">
+      <c r="K22" t="s">
+        <v>16</v>
+      </c>
+      <c r="L22" s="3">
         <v>218</v>
       </c>
+      <c r="M22">
+        <v>0.618389046</v>
+      </c>
       <c r="N22">
-        <v>0.618389046</v>
+        <v>966.66666669999995</v>
       </c>
       <c r="O22">
-        <v>966.66666669999995</v>
+        <v>6</v>
       </c>
       <c r="P22">
-        <v>6</v>
+        <v>228.15228830000001</v>
       </c>
       <c r="Q22">
-        <v>228.15228830000001</v>
-      </c>
-      <c r="R22">
         <v>3806.6326530000001</v>
       </c>
-      <c r="S22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>260</v>
       </c>
@@ -2272,49 +2203,46 @@
         <v>15.5</v>
       </c>
       <c r="F23">
-        <v>23</v>
-      </c>
-      <c r="G23">
         <v>1</v>
       </c>
-      <c r="H23" t="s">
-        <v>17</v>
+      <c r="G23" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23">
+        <v>189</v>
       </c>
       <c r="I23">
-        <v>189</v>
+        <v>0.63423868100000003</v>
       </c>
       <c r="J23">
-        <v>0.63423868100000003</v>
-      </c>
-      <c r="K23">
         <v>824.38461540000003</v>
       </c>
-      <c r="L23" t="s">
-        <v>17</v>
-      </c>
-      <c r="M23" s="3">
+      <c r="K23" t="s">
+        <v>16</v>
+      </c>
+      <c r="L23" s="3">
         <v>607</v>
       </c>
+      <c r="M23">
+        <v>0.66827764199999995</v>
+      </c>
       <c r="N23">
-        <v>0.66827764199999995</v>
+        <v>804.7857143</v>
       </c>
       <c r="O23">
-        <v>804.7857143</v>
+        <v>14</v>
       </c>
       <c r="P23">
-        <v>14</v>
+        <v>288.13463159999998</v>
       </c>
       <c r="Q23">
-        <v>288.13463159999998</v>
-      </c>
-      <c r="R23">
         <v>2587.6418659999999</v>
       </c>
-      <c r="S23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>308</v>
       </c>
@@ -2331,49 +2259,46 @@
         <v>30</v>
       </c>
       <c r="F24">
-        <v>30</v>
-      </c>
-      <c r="G24">
         <v>1</v>
       </c>
-      <c r="H24" t="s">
-        <v>17</v>
+      <c r="G24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24">
+        <v>14</v>
       </c>
       <c r="I24">
-        <v>14</v>
+        <v>0.64282002500000002</v>
       </c>
       <c r="J24">
-        <v>0.64282002500000002</v>
-      </c>
-      <c r="K24">
         <v>1019</v>
       </c>
-      <c r="L24" t="s">
-        <v>17</v>
-      </c>
-      <c r="M24" s="3">
+      <c r="K24" t="s">
+        <v>16</v>
+      </c>
+      <c r="L24" s="3">
         <v>94</v>
       </c>
+      <c r="M24">
+        <v>0.64880576099999998</v>
+      </c>
       <c r="N24">
-        <v>0.64880576099999998</v>
+        <v>842.55555560000005</v>
       </c>
       <c r="O24">
-        <v>842.55555560000005</v>
+        <v>9</v>
       </c>
       <c r="P24">
-        <v>9</v>
+        <v>315.34628229999998</v>
       </c>
       <c r="Q24">
-        <v>315.34628229999998</v>
-      </c>
-      <c r="R24">
         <v>1350</v>
       </c>
-      <c r="S24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>309</v>
       </c>
@@ -2390,49 +2315,46 @@
         <v>17</v>
       </c>
       <c r="F25">
-        <v>17</v>
-      </c>
-      <c r="G25">
         <v>1</v>
       </c>
-      <c r="H25" t="s">
-        <v>17</v>
+      <c r="G25" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25">
+        <v>12</v>
       </c>
       <c r="I25">
-        <v>12</v>
+        <v>0.429158551</v>
       </c>
       <c r="J25">
-        <v>0.429158551</v>
-      </c>
-      <c r="K25">
         <v>1316.75</v>
       </c>
-      <c r="L25" t="s">
-        <v>17</v>
-      </c>
-      <c r="M25" s="3">
+      <c r="K25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L25" s="3">
         <v>293</v>
       </c>
+      <c r="M25">
+        <v>0.49357283200000002</v>
+      </c>
       <c r="N25">
-        <v>0.49357283200000002</v>
+        <v>1060.25</v>
       </c>
       <c r="O25">
-        <v>1060.25</v>
+        <v>8</v>
       </c>
       <c r="P25">
-        <v>8</v>
+        <v>316.90816610000002</v>
       </c>
       <c r="Q25">
-        <v>316.90816610000002</v>
-      </c>
-      <c r="R25">
         <v>3148.2714470000001</v>
       </c>
-      <c r="S25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>310</v>
       </c>
@@ -2449,49 +2371,46 @@
         <v>22.5</v>
       </c>
       <c r="F26">
-        <v>25</v>
-      </c>
-      <c r="G26">
         <v>1</v>
       </c>
-      <c r="H26" t="s">
-        <v>17</v>
+      <c r="G26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26">
+        <v>230</v>
       </c>
       <c r="I26">
-        <v>230</v>
+        <v>0.56090952699999996</v>
       </c>
       <c r="J26">
-        <v>0.56090952699999996</v>
-      </c>
-      <c r="K26">
         <v>1066.636364</v>
       </c>
-      <c r="L26" t="s">
-        <v>17</v>
-      </c>
-      <c r="M26" s="3">
+      <c r="K26" t="s">
+        <v>16</v>
+      </c>
+      <c r="L26" s="3">
         <v>115</v>
       </c>
+      <c r="M26">
+        <v>0.72598247100000002</v>
+      </c>
       <c r="N26">
-        <v>0.72598247100000002</v>
+        <v>561.85714289999999</v>
       </c>
       <c r="O26">
-        <v>561.85714289999999</v>
+        <v>7</v>
       </c>
       <c r="P26">
-        <v>7</v>
+        <v>202.1801413</v>
       </c>
       <c r="Q26">
-        <v>202.1801413</v>
-      </c>
-      <c r="R26">
         <v>2456.3658839999998</v>
       </c>
-      <c r="S26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>351</v>
       </c>
@@ -2508,44 +2427,41 @@
         <v>27.5</v>
       </c>
       <c r="F27">
-        <v>29</v>
-      </c>
-      <c r="G27">
         <v>0</v>
       </c>
-      <c r="H27" t="s">
-        <v>17</v>
+      <c r="G27" t="s">
+        <v>16</v>
+      </c>
+      <c r="H27">
+        <v>36</v>
       </c>
       <c r="I27">
-        <v>36</v>
+        <v>0.57836958699999996</v>
       </c>
       <c r="J27">
-        <v>0.57836958699999996</v>
-      </c>
-      <c r="K27">
         <v>899.8</v>
       </c>
-      <c r="M27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27">
+        <v>0.591932558</v>
+      </c>
       <c r="N27">
-        <v>0.591932558</v>
+        <v>1124</v>
       </c>
       <c r="O27">
-        <v>1124</v>
+        <v>9</v>
       </c>
       <c r="P27">
-        <v>9</v>
+        <v>238.10449389999999</v>
       </c>
       <c r="Q27">
-        <v>238.10449389999999</v>
-      </c>
-      <c r="R27">
         <v>3103.4482760000001</v>
       </c>
-      <c r="S27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>354</v>
       </c>
@@ -2562,49 +2478,46 @@
         <v>16</v>
       </c>
       <c r="F28">
-        <v>20</v>
-      </c>
-      <c r="G28">
         <v>0</v>
       </c>
-      <c r="H28" t="s">
-        <v>17</v>
+      <c r="G28" t="s">
+        <v>16</v>
+      </c>
+      <c r="H28">
+        <v>458</v>
       </c>
       <c r="I28">
-        <v>458</v>
+        <v>0.55594844799999998</v>
       </c>
       <c r="J28">
-        <v>0.55594844799999998</v>
-      </c>
-      <c r="K28">
         <v>650</v>
       </c>
-      <c r="L28" t="s">
-        <v>17</v>
-      </c>
-      <c r="M28" s="3">
+      <c r="K28" t="s">
+        <v>16</v>
+      </c>
+      <c r="L28" s="3">
         <v>513</v>
       </c>
+      <c r="M28">
+        <v>0.44857279999999999</v>
+      </c>
       <c r="N28">
-        <v>0.44857279999999999</v>
+        <v>1230.7142859999999</v>
       </c>
       <c r="O28">
-        <v>1230.7142859999999</v>
+        <v>7</v>
       </c>
       <c r="P28">
-        <v>7</v>
+        <v>421.79011930000001</v>
       </c>
       <c r="Q28">
-        <v>421.79011930000001</v>
-      </c>
-      <c r="R28">
         <v>3626.9915649999998</v>
       </c>
-      <c r="S28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>355</v>
       </c>
@@ -2621,49 +2534,46 @@
         <v>27</v>
       </c>
       <c r="F29">
-        <v>30.5</v>
-      </c>
-      <c r="G29">
         <v>0</v>
       </c>
-      <c r="H29" t="s">
-        <v>17</v>
+      <c r="G29" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29">
+        <v>135</v>
       </c>
       <c r="I29">
-        <v>135</v>
+        <v>0.70391547399999999</v>
       </c>
       <c r="J29">
-        <v>0.70391547399999999</v>
-      </c>
-      <c r="K29">
         <v>829.25</v>
       </c>
-      <c r="L29" t="s">
-        <v>17</v>
-      </c>
-      <c r="M29" s="3">
+      <c r="K29" t="s">
+        <v>16</v>
+      </c>
+      <c r="L29" s="3">
         <v>164</v>
       </c>
+      <c r="M29">
+        <v>0.66095326600000004</v>
+      </c>
       <c r="N29">
-        <v>0.66095326600000004</v>
+        <v>761.33333330000005</v>
       </c>
       <c r="O29">
-        <v>761.33333330000005</v>
+        <v>3</v>
       </c>
       <c r="P29">
-        <v>3</v>
+        <v>58.705479590000003</v>
       </c>
       <c r="Q29">
-        <v>58.705479590000003</v>
-      </c>
-      <c r="R29">
         <v>3940</v>
       </c>
-      <c r="S29" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>369</v>
       </c>
@@ -2680,49 +2590,46 @@
         <v>18.5</v>
       </c>
       <c r="F30">
-        <v>20</v>
-      </c>
-      <c r="G30">
         <v>0</v>
       </c>
-      <c r="H30" t="s">
-        <v>17</v>
+      <c r="G30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30">
+        <v>8</v>
       </c>
       <c r="I30">
-        <v>8</v>
+        <v>0.565917208</v>
       </c>
       <c r="J30">
-        <v>0.565917208</v>
-      </c>
-      <c r="K30">
         <v>1115.181818</v>
       </c>
-      <c r="L30" t="s">
-        <v>17</v>
-      </c>
-      <c r="M30" s="3">
+      <c r="K30" t="s">
+        <v>16</v>
+      </c>
+      <c r="L30" s="3">
         <v>174</v>
       </c>
+      <c r="M30">
+        <v>0.59022613300000004</v>
+      </c>
       <c r="N30">
-        <v>0.59022613300000004</v>
+        <v>939.47368419999998</v>
       </c>
       <c r="O30">
-        <v>939.47368419999998</v>
+        <v>19</v>
       </c>
       <c r="P30">
-        <v>19</v>
+        <v>333.94450110000002</v>
       </c>
       <c r="Q30">
-        <v>333.94450110000002</v>
-      </c>
-      <c r="R30">
         <v>3458.8878759999998</v>
       </c>
-      <c r="S30" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>370</v>
       </c>
@@ -2739,49 +2646,46 @@
         <v>8</v>
       </c>
       <c r="F31">
-        <v>12</v>
-      </c>
-      <c r="G31">
         <v>0</v>
       </c>
-      <c r="H31" t="s">
-        <v>17</v>
+      <c r="G31" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31">
+        <v>40</v>
       </c>
       <c r="I31">
-        <v>40</v>
+        <v>0.55720972400000002</v>
       </c>
       <c r="J31">
-        <v>0.55720972400000002</v>
-      </c>
-      <c r="K31">
         <v>783</v>
       </c>
-      <c r="L31" t="s">
-        <v>17</v>
-      </c>
-      <c r="M31" s="3">
+      <c r="K31" t="s">
+        <v>16</v>
+      </c>
+      <c r="L31" s="3">
         <v>154</v>
       </c>
+      <c r="M31">
+        <v>0.59181818200000003</v>
+      </c>
       <c r="N31">
-        <v>0.59181818200000003</v>
+        <v>983</v>
       </c>
       <c r="O31">
-        <v>983</v>
+        <v>2</v>
       </c>
       <c r="P31">
-        <v>2</v>
+        <v>212.13203440000001</v>
       </c>
       <c r="Q31">
-        <v>212.13203440000001</v>
-      </c>
-      <c r="R31">
         <v>3634.6820809999999</v>
       </c>
-      <c r="S31" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>372</v>
       </c>
@@ -2798,49 +2702,46 @@
         <v>25</v>
       </c>
       <c r="F32">
-        <v>19</v>
-      </c>
-      <c r="G32">
         <v>1</v>
       </c>
-      <c r="H32" t="s">
-        <v>17</v>
+      <c r="G32" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32">
+        <v>20</v>
       </c>
       <c r="I32">
-        <v>20</v>
+        <v>0.82250660399999997</v>
       </c>
       <c r="J32">
-        <v>0.82250660399999997</v>
-      </c>
-      <c r="K32">
         <v>566.66666669999995</v>
       </c>
-      <c r="L32" t="s">
-        <v>17</v>
-      </c>
-      <c r="M32" s="3">
+      <c r="K32" t="s">
+        <v>16</v>
+      </c>
+      <c r="L32" s="3">
         <v>139</v>
       </c>
+      <c r="M32">
+        <v>0.560303832</v>
+      </c>
       <c r="N32">
-        <v>0.560303832</v>
+        <v>736.16666669999995</v>
       </c>
       <c r="O32">
-        <v>736.16666669999995</v>
+        <v>12</v>
       </c>
       <c r="P32">
-        <v>12</v>
+        <v>302.6422531</v>
       </c>
       <c r="Q32">
-        <v>302.6422531</v>
-      </c>
-      <c r="R32">
         <v>4055.1330800000001</v>
       </c>
-      <c r="S32" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>400</v>
       </c>
@@ -2857,49 +2758,46 @@
         <v>18</v>
       </c>
       <c r="F33">
-        <v>13</v>
-      </c>
-      <c r="G33">
         <v>1</v>
       </c>
-      <c r="H33" t="s">
-        <v>17</v>
-      </c>
-      <c r="I33" s="3">
+      <c r="G33" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="3">
         <v>57</v>
       </c>
+      <c r="I33">
+        <v>0.610823911</v>
+      </c>
       <c r="J33">
-        <v>0.610823911</v>
-      </c>
-      <c r="K33">
         <v>858.33333330000005</v>
       </c>
-      <c r="L33" t="s">
-        <v>17</v>
-      </c>
-      <c r="M33" s="3">
+      <c r="K33" t="s">
+        <v>16</v>
+      </c>
+      <c r="L33" s="3">
         <v>330</v>
       </c>
+      <c r="M33">
+        <v>0.54962503299999999</v>
+      </c>
       <c r="N33">
-        <v>0.54962503299999999</v>
+        <v>820.2</v>
       </c>
       <c r="O33">
-        <v>820.2</v>
+        <v>5</v>
       </c>
       <c r="P33">
-        <v>5</v>
+        <v>432.00891189999999</v>
       </c>
       <c r="Q33">
-        <v>432.00891189999999</v>
-      </c>
-      <c r="R33">
         <v>2664</v>
       </c>
-      <c r="S33" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>401</v>
       </c>
@@ -2916,39 +2814,36 @@
         <v>20</v>
       </c>
       <c r="F34">
-        <v>21.5</v>
-      </c>
-      <c r="G34">
         <v>1</v>
       </c>
-      <c r="I34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34">
+        <v>0.58468254200000003</v>
+      </c>
       <c r="J34">
-        <v>0.58468254200000003</v>
-      </c>
-      <c r="K34">
         <v>928.57142859999999</v>
       </c>
-      <c r="M34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34">
+        <v>0.72300366900000002</v>
+      </c>
       <c r="N34">
-        <v>0.72300366900000002</v>
+        <v>798.63636359999998</v>
       </c>
       <c r="O34">
-        <v>798.63636359999998</v>
+        <v>11</v>
       </c>
       <c r="P34">
-        <v>11</v>
+        <v>385.56199830000003</v>
       </c>
       <c r="Q34">
-        <v>385.56199830000003</v>
-      </c>
-      <c r="R34">
         <v>5160.1756949999999</v>
       </c>
-      <c r="S34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>411</v>
       </c>
@@ -2965,44 +2860,41 @@
         <v>54.5</v>
       </c>
       <c r="F35">
-        <v>54.5</v>
-      </c>
-      <c r="G35">
         <v>1</v>
       </c>
-      <c r="I35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35">
+        <v>0.70533375700000001</v>
+      </c>
       <c r="J35">
-        <v>0.70533375700000001</v>
-      </c>
-      <c r="K35">
         <v>751.88888889999998</v>
       </c>
-      <c r="L35" t="s">
-        <v>17</v>
-      </c>
-      <c r="M35" s="3">
+      <c r="K35" t="s">
+        <v>16</v>
+      </c>
+      <c r="L35" s="3">
         <v>305</v>
       </c>
+      <c r="M35">
+        <v>0.70066277399999999</v>
+      </c>
       <c r="N35">
-        <v>0.70066277399999999</v>
+        <v>733.4</v>
       </c>
       <c r="O35">
-        <v>733.4</v>
+        <v>5</v>
       </c>
       <c r="P35">
-        <v>5</v>
+        <v>282.60714780000001</v>
       </c>
       <c r="Q35">
-        <v>282.60714780000001</v>
-      </c>
-      <c r="R35">
         <v>1752</v>
       </c>
-      <c r="S35" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>414</v>
       </c>
@@ -3019,49 +2911,46 @@
         <v>23.5</v>
       </c>
       <c r="F36">
-        <v>38.5</v>
-      </c>
-      <c r="G36">
         <v>0</v>
       </c>
-      <c r="H36" t="s">
-        <v>17</v>
-      </c>
-      <c r="I36" s="3">
+      <c r="G36" t="s">
+        <v>16</v>
+      </c>
+      <c r="H36" s="3">
         <v>28</v>
       </c>
+      <c r="I36">
+        <v>0.53346854700000002</v>
+      </c>
       <c r="J36">
-        <v>0.53346854700000002</v>
-      </c>
-      <c r="K36">
         <v>1172.333333</v>
       </c>
-      <c r="L36" t="s">
-        <v>17</v>
-      </c>
-      <c r="M36" s="3">
+      <c r="K36" t="s">
+        <v>16</v>
+      </c>
+      <c r="L36" s="3">
         <v>178</v>
       </c>
+      <c r="M36">
+        <v>0.62326193799999996</v>
+      </c>
       <c r="N36">
-        <v>0.62326193799999996</v>
+        <v>1204.25</v>
       </c>
       <c r="O36">
-        <v>1204.25</v>
+        <v>4</v>
       </c>
       <c r="P36">
-        <v>4</v>
+        <v>270.87312530000003</v>
       </c>
       <c r="Q36">
-        <v>270.87312530000003</v>
-      </c>
-      <c r="R36">
         <v>925.13966479999999</v>
       </c>
-      <c r="S36" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>415</v>
       </c>
@@ -3078,49 +2967,46 @@
         <v>59</v>
       </c>
       <c r="F37">
-        <v>59</v>
-      </c>
-      <c r="G37">
         <v>0</v>
       </c>
-      <c r="H37" t="s">
-        <v>17</v>
+      <c r="G37" t="s">
+        <v>16</v>
+      </c>
+      <c r="H37">
+        <v>7</v>
       </c>
       <c r="I37">
-        <v>7</v>
+        <v>0.467875612</v>
       </c>
       <c r="J37">
-        <v>0.467875612</v>
-      </c>
-      <c r="K37">
         <v>1160.2</v>
       </c>
-      <c r="L37" t="s">
-        <v>17</v>
+      <c r="K37" t="s">
+        <v>16</v>
+      </c>
+      <c r="L37">
+        <v>134</v>
       </c>
       <c r="M37">
-        <v>134</v>
+        <v>0.52042339299999996</v>
       </c>
       <c r="N37">
-        <v>0.52042339299999996</v>
+        <v>1161</v>
       </c>
       <c r="O37">
-        <v>1161</v>
+        <v>6</v>
       </c>
       <c r="P37">
-        <v>6</v>
+        <v>335.51512630000002</v>
       </c>
       <c r="Q37">
-        <v>335.51512630000002</v>
-      </c>
-      <c r="R37">
         <v>1508.0394920000001</v>
       </c>
-      <c r="S37" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>417</v>
       </c>
@@ -3137,49 +3023,46 @@
         <v>62</v>
       </c>
       <c r="F38">
-        <v>62</v>
-      </c>
-      <c r="G38">
         <v>1</v>
       </c>
-      <c r="H38" t="s">
-        <v>17</v>
+      <c r="G38" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38">
+        <v>329</v>
       </c>
       <c r="I38">
-        <v>329</v>
+        <v>0.55166093500000002</v>
       </c>
       <c r="J38">
-        <v>0.55166093500000002</v>
-      </c>
-      <c r="K38">
         <v>1060</v>
       </c>
-      <c r="L38" t="s">
-        <v>17</v>
+      <c r="K38" t="s">
+        <v>16</v>
+      </c>
+      <c r="L38">
+        <v>536</v>
       </c>
       <c r="M38">
-        <v>536</v>
+        <v>0.68455337400000005</v>
       </c>
       <c r="N38">
-        <v>0.68455337400000005</v>
+        <v>809.42857140000001</v>
       </c>
       <c r="O38">
-        <v>809.42857140000001</v>
+        <v>7</v>
       </c>
       <c r="P38">
-        <v>7</v>
+        <v>181.94949589999999</v>
       </c>
       <c r="Q38">
-        <v>181.94949589999999</v>
-      </c>
-      <c r="R38">
         <v>5388</v>
       </c>
-      <c r="S38" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R38" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>431</v>
       </c>
@@ -3196,49 +3079,46 @@
         <v>29</v>
       </c>
       <c r="F39">
-        <v>29</v>
-      </c>
-      <c r="G39">
         <v>0</v>
       </c>
-      <c r="H39" t="s">
-        <v>17</v>
+      <c r="G39" t="s">
+        <v>16</v>
+      </c>
+      <c r="H39">
+        <v>18</v>
       </c>
       <c r="I39">
-        <v>18</v>
+        <v>0.55619865000000002</v>
       </c>
       <c r="J39">
-        <v>0.55619865000000002</v>
-      </c>
-      <c r="K39">
         <v>827.83333330000005</v>
       </c>
-      <c r="L39" t="s">
-        <v>17</v>
+      <c r="K39" t="s">
+        <v>16</v>
+      </c>
+      <c r="L39">
+        <v>258</v>
       </c>
       <c r="M39">
-        <v>258</v>
+        <v>0.69612368899999999</v>
       </c>
       <c r="N39">
-        <v>0.69612368899999999</v>
+        <v>721.18181819999995</v>
       </c>
       <c r="O39">
-        <v>721.18181819999995</v>
+        <v>11</v>
       </c>
       <c r="P39">
-        <v>11</v>
+        <v>181.41379119999999</v>
       </c>
       <c r="Q39">
-        <v>181.41379119999999</v>
-      </c>
-      <c r="R39">
         <v>6683.3836860000001</v>
       </c>
-      <c r="S39" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>433</v>
       </c>
@@ -3255,49 +3135,46 @@
         <v>22</v>
       </c>
       <c r="F40">
-        <v>22</v>
-      </c>
-      <c r="G40">
         <v>0</v>
       </c>
-      <c r="H40" t="s">
-        <v>17</v>
+      <c r="G40" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40">
+        <v>100</v>
       </c>
       <c r="I40">
-        <v>100</v>
+        <v>0.583681911</v>
       </c>
       <c r="J40">
-        <v>0.583681911</v>
-      </c>
-      <c r="K40">
         <v>748.36363640000002</v>
       </c>
-      <c r="L40" t="s">
-        <v>17</v>
+      <c r="K40" t="s">
+        <v>16</v>
+      </c>
+      <c r="L40">
+        <v>351</v>
       </c>
       <c r="M40">
-        <v>351</v>
+        <v>0.58690365200000005</v>
       </c>
       <c r="N40">
-        <v>0.58690365200000005</v>
+        <v>886.16666669999995</v>
       </c>
       <c r="O40">
-        <v>886.16666669999995</v>
+        <v>6</v>
       </c>
       <c r="P40">
-        <v>6</v>
+        <v>392.5803952</v>
       </c>
       <c r="Q40">
-        <v>392.5803952</v>
-      </c>
-      <c r="R40">
         <v>1374.6397689999999</v>
       </c>
-      <c r="S40" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R40" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>436</v>
       </c>
@@ -3313,50 +3190,47 @@
       <c r="E41">
         <v>22.5</v>
       </c>
-      <c r="F41">
-        <v>15.5</v>
-      </c>
-      <c r="G41" s="3">
+      <c r="F41" s="3">
         <v>0</v>
       </c>
-      <c r="H41" s="3" t="s">
-        <v>17</v>
+      <c r="G41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="3">
+        <v>46</v>
       </c>
       <c r="I41" s="3">
-        <v>46</v>
+        <v>0.71203714100000004</v>
       </c>
       <c r="J41" s="3">
-        <v>0.71203714100000004</v>
-      </c>
-      <c r="K41" s="3">
         <v>650</v>
       </c>
-      <c r="L41" s="3" t="s">
-        <v>17</v>
+      <c r="K41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L41" s="3">
+        <v>77</v>
       </c>
       <c r="M41" s="3">
-        <v>77</v>
+        <v>0.78</v>
       </c>
       <c r="N41" s="3">
-        <v>0.78</v>
+        <v>577.66999999999996</v>
       </c>
       <c r="O41" s="3">
-        <v>577.66999999999996</v>
+        <v>3</v>
       </c>
       <c r="P41" s="3">
-        <v>3</v>
-      </c>
-      <c r="Q41" s="3">
         <v>234.29966569999999</v>
       </c>
-      <c r="R41">
+      <c r="Q41">
         <v>3695.4344620000002</v>
       </c>
-      <c r="S41" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R41" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>444</v>
       </c>
@@ -3372,50 +3246,47 @@
       <c r="E42">
         <v>28</v>
       </c>
-      <c r="F42">
-        <v>28</v>
-      </c>
-      <c r="G42" s="3">
+      <c r="F42" s="3">
         <v>1</v>
       </c>
-      <c r="H42" s="3" t="s">
-        <v>17</v>
+      <c r="G42" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H42" s="3">
+        <v>15</v>
       </c>
       <c r="I42" s="3">
-        <v>15</v>
+        <v>0.54545390000000005</v>
       </c>
       <c r="J42" s="3">
-        <v>0.54545390000000005</v>
-      </c>
-      <c r="K42" s="3">
         <v>672.16666669999995</v>
       </c>
-      <c r="L42" s="3" t="s">
-        <v>17</v>
+      <c r="K42" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L42" s="3">
+        <v>14</v>
       </c>
       <c r="M42" s="3">
-        <v>14</v>
+        <v>0.6</v>
       </c>
       <c r="N42" s="3">
-        <v>0.6</v>
+        <v>636.70000000000005</v>
       </c>
       <c r="O42" s="3">
-        <v>636.70000000000005</v>
+        <v>10</v>
       </c>
       <c r="P42" s="3">
-        <v>10</v>
-      </c>
-      <c r="Q42" s="3">
         <v>222.09409919999999</v>
       </c>
-      <c r="R42">
+      <c r="Q42">
         <v>2955</v>
       </c>
-      <c r="S42" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R42" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>445</v>
       </c>
@@ -3431,47 +3302,44 @@
       <c r="E43">
         <v>24</v>
       </c>
-      <c r="F43">
-        <v>21.5</v>
-      </c>
-      <c r="G43" s="3">
+      <c r="F43" s="3">
         <v>0</v>
       </c>
-      <c r="H43" s="3" t="s">
-        <v>17</v>
+      <c r="G43" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H43" s="3">
+        <v>73</v>
       </c>
       <c r="I43" s="3">
-        <v>73</v>
+        <v>0.450199866</v>
       </c>
       <c r="J43" s="3">
-        <v>0.450199866</v>
-      </c>
-      <c r="K43" s="3">
         <v>820.75</v>
       </c>
-      <c r="L43" s="3" t="s">
-        <v>17</v>
+      <c r="K43" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L43" s="3">
+        <v>270</v>
       </c>
       <c r="M43" s="3">
-        <v>270</v>
+        <v>0.72</v>
       </c>
       <c r="N43" s="3">
-        <v>0.72</v>
-      </c>
-      <c r="O43" s="3">
         <v>860.2</v>
       </c>
+      <c r="O43">
+        <v>10</v>
+      </c>
       <c r="P43">
-        <v>10</v>
+        <v>252.4972167</v>
       </c>
       <c r="Q43">
-        <v>252.4972167</v>
-      </c>
-      <c r="R43">
         <v>531.94029850000004</v>
       </c>
-      <c r="S43" t="s">
-        <v>21</v>
+      <c r="R43" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>